<commit_message>
Get rid of svn files
</commit_message>
<xml_diff>
--- a/555-prototyper-v2/price-breaks-sep-21-2015.xlsx
+++ b/555-prototyper-v2/price-breaks-sep-21-2015.xlsx
@@ -35,16 +35,16 @@
     <t>BULK</t>
   </si>
   <si>
-    <t>LIGHT BULK</t>
-  </si>
-  <si>
     <t>NONBULK</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>**Note: Shipping charges for the NONBULK category have been factored into the price, however some extra shipping charges will apply to the LIGHT BULK and BULK categories which you will be notified about after purchase</t>
+    <t>**Note: Shipping charges for the NONBULK category have been factored into the price, however some extra shipping charges will apply to the BULK category which we will communicate to you shortly before shipping your order</t>
+  </si>
+  <si>
+    <t>Additionally, every order will come with enough pink plastic ESD bags to hold all of the boards ordered, however the boards will only be bagged individually for NONBULK orders</t>
   </si>
 </sst>
 </file>
@@ -88,12 +88,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,21 +375,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -395,14 +399,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -415,6 +419,7 @@
       <c r="C3" s="2">
         <v>1197.33</v>
       </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -426,6 +431,7 @@
       <c r="C4" s="2">
         <v>655.26</v>
       </c>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -437,6 +443,7 @@
       <c r="C5" s="2">
         <v>533.89</v>
       </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -448,103 +455,104 @@
       <c r="C6" s="2">
         <v>376.51</v>
       </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="1">
+        <v>125</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="C7" s="2">
+        <v>226.25</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2">
-        <v>1.81</v>
+        <v>1.91</v>
       </c>
       <c r="C8" s="2">
-        <v>226.25</v>
+        <v>114.78</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
-        <v>1.91</v>
+        <v>2.02</v>
       </c>
       <c r="C9" s="2">
-        <v>114.78</v>
-      </c>
+        <v>60.48</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.02</v>
-      </c>
-      <c r="C10" s="2">
-        <v>60.48</v>
-      </c>
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="C11" s="2">
+        <v>42.31</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>4.2300000000000004</v>
+        <v>4.49</v>
       </c>
       <c r="C12" s="2">
-        <v>42.31</v>
+        <v>22.44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
-        <v>4.49</v>
+        <v>5.35</v>
       </c>
       <c r="C13" s="2">
-        <v>22.44</v>
+        <v>10.71</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2">
-        <v>5.35</v>
+        <v>5.92</v>
       </c>
       <c r="C14" s="2">
-        <v>10.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
         <v>5.92</v>
       </c>
-      <c r="C15" s="2">
-        <v>5.92</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="E8:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>